<commit_message>
ADD: prius CNG: citycar
</commit_message>
<xml_diff>
--- a/Source/Japanese_city_car_source/citycar/citycar.xlsx
+++ b/Source/Japanese_city_car_source/citycar/citycar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anok1\Documents\GitHub\simutrans-extended_Japansese_city_car\Source\Japanese_city_car_source\citycar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B300F0E0-27DB-4DC9-9889-E85451B09BFE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B918A4A-10DE-4BBA-8768-990F67EAE758}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="141">
   <si>
     <t>datname</t>
     <phoneticPr fontId="1"/>
@@ -544,10 +544,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>../images/OBKcars02</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>#citycar/dat/Japansese_city_car.dat</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -589,6 +585,24 @@
   </si>
   <si>
     <t>citycar</t>
+  </si>
+  <si>
+    <t>../images/brius</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Harucarro</t>
+  </si>
+  <si>
+    <t>TODOYA-Brius-1</t>
+  </si>
+  <si>
+    <t>TODOYA-Brius-2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>../images/OBKcars002</t>
+    <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
@@ -924,10 +938,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T24"/>
+  <dimension ref="A1:T27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>
@@ -948,7 +962,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -1061,7 +1075,7 @@
         <v>30</v>
       </c>
       <c r="D5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E5" t="s">
         <v>29</v>
@@ -1114,7 +1128,7 @@
         <v>31</v>
       </c>
       <c r="D6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E6" t="s">
         <v>29</v>
@@ -1167,7 +1181,7 @@
         <v>32</v>
       </c>
       <c r="D7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E7" t="s">
         <v>29</v>
@@ -1220,7 +1234,7 @@
         <v>33</v>
       </c>
       <c r="D8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E8" t="s">
         <v>29</v>
@@ -1273,7 +1287,7 @@
         <v>34</v>
       </c>
       <c r="D9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E9" t="s">
         <v>29</v>
@@ -1326,7 +1340,7 @@
         <v>35</v>
       </c>
       <c r="D10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E10" t="s">
         <v>29</v>
@@ -1379,7 +1393,7 @@
         <v>36</v>
       </c>
       <c r="D11" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E11" t="s">
         <v>29</v>
@@ -1438,7 +1452,7 @@
         <v>37</v>
       </c>
       <c r="D12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E12" t="s">
         <v>29</v>
@@ -1497,7 +1511,7 @@
         <v>38</v>
       </c>
       <c r="D13" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E13" t="s">
         <v>29</v>
@@ -1550,7 +1564,7 @@
         <v>106</v>
       </c>
       <c r="D14" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E14" t="s">
         <v>29</v>
@@ -1603,13 +1617,13 @@
     </row>
     <row r="15" spans="1:20">
       <c r="A15" t="s">
-        <v>126</v>
+        <v>28</v>
       </c>
       <c r="C15" t="s">
         <v>115</v>
       </c>
       <c r="D15" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E15" t="s">
         <v>29</v>
@@ -1624,7 +1638,7 @@
         <v>1951</v>
       </c>
       <c r="L15" t="s">
-        <v>125</v>
+        <v>140</v>
       </c>
       <c r="M15" s="2" t="s">
         <v>42</v>
@@ -1653,13 +1667,13 @@
     </row>
     <row r="16" spans="1:20">
       <c r="A16" t="s">
-        <v>126</v>
+        <v>28</v>
       </c>
       <c r="C16" t="s">
         <v>116</v>
       </c>
       <c r="D16" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E16" t="s">
         <v>29</v>
@@ -1674,7 +1688,7 @@
         <v>1951</v>
       </c>
       <c r="L16" t="s">
-        <v>125</v>
+        <v>140</v>
       </c>
       <c r="M16" s="2" t="s">
         <v>50</v>
@@ -1703,13 +1717,13 @@
     </row>
     <row r="17" spans="1:20">
       <c r="A17" t="s">
-        <v>126</v>
+        <v>28</v>
       </c>
       <c r="C17" t="s">
         <v>117</v>
       </c>
       <c r="D17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E17" t="s">
         <v>29</v>
@@ -1724,7 +1738,7 @@
         <v>1951</v>
       </c>
       <c r="L17" t="s">
-        <v>125</v>
+        <v>140</v>
       </c>
       <c r="M17" s="2" t="s">
         <v>65</v>
@@ -1753,13 +1767,13 @@
     </row>
     <row r="18" spans="1:20">
       <c r="A18" t="s">
-        <v>126</v>
+        <v>28</v>
       </c>
       <c r="C18" t="s">
         <v>118</v>
       </c>
       <c r="D18" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E18" t="s">
         <v>29</v>
@@ -1774,7 +1788,7 @@
         <v>1951</v>
       </c>
       <c r="L18" t="s">
-        <v>125</v>
+        <v>140</v>
       </c>
       <c r="M18" s="2" t="s">
         <v>66</v>
@@ -1803,13 +1817,13 @@
     </row>
     <row r="19" spans="1:20">
       <c r="A19" t="s">
-        <v>126</v>
-      </c>
-      <c r="C19" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>119</v>
       </c>
       <c r="D19" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E19" t="s">
         <v>29</v>
@@ -1824,7 +1838,7 @@
         <v>1951</v>
       </c>
       <c r="L19" t="s">
-        <v>125</v>
+        <v>140</v>
       </c>
       <c r="M19" s="2" t="s">
         <v>74</v>
@@ -1853,13 +1867,13 @@
     </row>
     <row r="20" spans="1:20">
       <c r="A20" t="s">
-        <v>126</v>
+        <v>28</v>
       </c>
       <c r="C20" t="s">
         <v>120</v>
       </c>
       <c r="D20" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E20" t="s">
         <v>29</v>
@@ -1874,7 +1888,7 @@
         <v>1951</v>
       </c>
       <c r="L20" t="s">
-        <v>125</v>
+        <v>140</v>
       </c>
       <c r="M20" s="2" t="s">
         <v>82</v>
@@ -1903,13 +1917,13 @@
     </row>
     <row r="21" spans="1:20">
       <c r="A21" t="s">
-        <v>126</v>
+        <v>28</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>121</v>
       </c>
       <c r="D21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E21" t="s">
         <v>29</v>
@@ -1924,7 +1938,7 @@
         <v>1951</v>
       </c>
       <c r="L21" t="s">
-        <v>125</v>
+        <v>140</v>
       </c>
       <c r="M21" s="2" t="s">
         <v>90</v>
@@ -1953,13 +1967,13 @@
     </row>
     <row r="22" spans="1:20">
       <c r="A22" t="s">
-        <v>126</v>
+        <v>28</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>122</v>
       </c>
       <c r="D22" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E22" t="s">
         <v>29</v>
@@ -1974,7 +1988,7 @@
         <v>1951</v>
       </c>
       <c r="L22" t="s">
-        <v>125</v>
+        <v>140</v>
       </c>
       <c r="M22" s="2" t="s">
         <v>98</v>
@@ -2003,13 +2017,13 @@
     </row>
     <row r="23" spans="1:20">
       <c r="A23" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>123</v>
       </c>
       <c r="D23" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E23" t="s">
         <v>29</v>
@@ -2024,7 +2038,7 @@
         <v>1951</v>
       </c>
       <c r="L23" t="s">
-        <v>125</v>
+        <v>140</v>
       </c>
       <c r="M23" s="2" t="s">
         <v>107</v>
@@ -2053,13 +2067,13 @@
     </row>
     <row r="24" spans="1:20">
       <c r="A24" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>124</v>
       </c>
       <c r="D24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E24" t="s">
         <v>29</v>
@@ -2074,31 +2088,137 @@
         <v>1951</v>
       </c>
       <c r="L24" t="s">
-        <v>125</v>
+        <v>140</v>
       </c>
       <c r="M24" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="N24" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="N24" s="2" t="s">
+      <c r="O24" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="O24" s="2" t="s">
+      <c r="P24" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="P24" s="2" t="s">
+      <c r="Q24" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="Q24" s="2" t="s">
+      <c r="R24" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="R24" s="2" t="s">
+      <c r="S24" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="S24" s="2" t="s">
+      <c r="T24" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="T24" s="2" t="s">
-        <v>134</v>
+    </row>
+    <row r="26" spans="1:20">
+      <c r="A26" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26" t="s">
+        <v>138</v>
+      </c>
+      <c r="D26" t="s">
+        <v>135</v>
+      </c>
+      <c r="E26" t="s">
+        <v>137</v>
+      </c>
+      <c r="F26">
+        <v>135</v>
+      </c>
+      <c r="G26">
+        <v>11</v>
+      </c>
+      <c r="H26">
+        <v>2011</v>
+      </c>
+      <c r="I26">
+        <v>10</v>
+      </c>
+      <c r="L26" t="s">
+        <v>136</v>
+      </c>
+      <c r="M26" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N26" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="O26" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="P26" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q26" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="R26" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="S26" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="T26" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20">
+      <c r="A27" t="s">
+        <v>28</v>
+      </c>
+      <c r="C27" t="s">
+        <v>139</v>
+      </c>
+      <c r="D27" t="s">
+        <v>135</v>
+      </c>
+      <c r="E27" t="s">
+        <v>137</v>
+      </c>
+      <c r="F27">
+        <v>130</v>
+      </c>
+      <c r="G27">
+        <v>9</v>
+      </c>
+      <c r="H27">
+        <v>2011</v>
+      </c>
+      <c r="I27">
+        <v>11</v>
+      </c>
+      <c r="L27" t="s">
+        <v>136</v>
+      </c>
+      <c r="M27" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="N27" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="O27" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="P27" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q27" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="R27" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="S27" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="T27" s="2" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>